<commit_message>
Add SQL script to fetch last non-null values from footer table
</commit_message>
<xml_diff>
--- a/Fetch_Footer_Values/Problem_Statement.xlsx
+++ b/Fetch_Footer_Values/Problem_Statement.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thoufiq/THOUFIQ/techTFQ/YouTube/VIDEOS/30 SQL Interview Queries/Video_Q3/Video_Q3_Scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\30DaySQLQueryChallenge - techTFQ\Fetch_Footer_Values\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA4D26A-E92C-4A43-B06B-A42E6FDDA820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F93439-F792-4B69-9130-EE30C0551C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{F52B1AC0-829F-0D4F-9731-C4603F8BFC93}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{F52B1AC0-829F-0D4F-9731-C4603F8BFC93}"/>
   </bookViews>
   <sheets>
     <sheet name="Video Q3" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -91,7 +89,7 @@
   </si>
   <si>
     <r>
-      <t>Video #3 -</t>
+      <t># -</t>
     </r>
     <r>
       <rPr>
@@ -837,20 +835,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC654931-91D8-F346-84BB-522F9548E124}">
   <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="2" max="2" width="10.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.83203125" style="1" customWidth="1"/>
-    <col min="4" max="6" width="10.83203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="10.796875" style="1"/>
+    <col min="2" max="2" width="10.796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.796875" style="1" customWidth="1"/>
+    <col min="4" max="6" width="10.796875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="29" t="s">
         <v>11</v>
       </c>
@@ -866,7 +864,7 @@
       <c r="K1" s="29"/>
       <c r="L1" s="29"/>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="28" t="s">
         <v>10</v>
       </c>
@@ -880,7 +878,7 @@
       <c r="J2" s="28"/>
       <c r="K2" s="28"/>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
@@ -892,7 +890,7 @@
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="28"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -904,8 +902,8 @@
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="6" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="25" t="s">
         <v>8</v>
       </c>
@@ -914,7 +912,7 @@
       <c r="E6" s="26"/>
       <c r="F6" s="27"/>
     </row>
-    <row r="7" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
@@ -931,7 +929,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B8" s="6">
         <v>1</v>
       </c>
@@ -946,7 +944,7 @@
       </c>
       <c r="F8" s="9"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B9" s="18">
         <v>2</v>
       </c>
@@ -957,7 +955,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B10" s="10">
         <v>3</v>
       </c>
@@ -972,7 +970,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B11" s="18">
         <v>4</v>
       </c>
@@ -985,7 +983,7 @@
       </c>
       <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="14">
         <v>5</v>
       </c>
@@ -998,8 +996,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="15" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C15" s="25" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1005,7 @@
       <c r="E15" s="26"/>
       <c r="F15" s="27"/>
     </row>
-    <row r="16" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1021,7 +1019,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="3:6" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:6" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C17" s="22" t="s">
         <v>2</v>
       </c>
@@ -1043,5 +1041,6 @@
     <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>